<commit_message>
Untrack .emf and .tif
</commit_message>
<xml_diff>
--- a/nom_fichiers.xlsx
+++ b/nom_fichiers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\PRI\enregistrements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843DD38C-3227-4ED5-8F5F-E89545FA51AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE0B9A4-9A5F-43C2-B7C7-FDA0C3A44396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="776">
   <si>
     <t>test_FxFy_perlite_1</t>
   </si>
@@ -1144,6 +1144,1215 @@
   </si>
   <si>
     <t>incertitude_WEL_30</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_1</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_2</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_3</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_4</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_5</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_6</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_7</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_8</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_9</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_10</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_11</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_12</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_13</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_14</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_15</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_16</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_17</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_18</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_19</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_20</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_21</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_22</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_23</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_24</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_25</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_26</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_27</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_28</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_29</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_30</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_31</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_32</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_33</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_34</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_35</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_36</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_37</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_38</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_39</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_40</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_41</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_42</t>
+  </si>
+  <si>
+    <t>benchmarks_perlite_rug_43</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_1</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_2</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_3</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_4</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_5</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_6</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_7</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_8</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_9</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_10</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_11</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_12</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_13</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_14</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_15</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_16</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_17</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_18</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_19</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_20</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_21</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_22</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_23</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_24</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_25</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_26</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_27</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_28</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_29</t>
+  </si>
+  <si>
+    <t>benchmarks_martensitev2_30</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_1</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_6</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_2</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_3</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_4</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_5</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_6</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_7</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_8</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_9</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_10</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_11</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_12</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_13</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_14</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_15</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_16</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_17</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_18</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_19</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_20</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_21</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_22</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_23</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_24</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_25</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_26</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_27</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_28</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_29</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1I_30</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_1</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_2</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_3</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_4</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_5</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_6</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_7</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_8</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_9</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_10</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_11</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_12</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_13</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_14</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_15</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_16</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_17</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_18</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_19</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_20</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_21</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_22</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_23</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_24</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_25</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_26</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_27</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_28</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_29</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1II_30</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_1</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_2</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_3</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_4</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_5</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_6</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_7</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_8</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_9</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_10</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_11</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_12</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_13</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_14</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_15</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_16</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_17</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_18</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_19</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_20</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_21</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_22</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_23</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_24</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_25</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_26</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_27</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_28</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_29</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1III_30</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_1</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_2</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_3</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_4</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_5</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_6</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_7</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_8</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_9</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_10</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_11</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_12</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_13</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_14</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_15</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_16</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_17</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_18</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_19</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_20</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_21</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_22</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_23</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_24</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_25</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_26</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_27</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_28</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_29</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC1IV_30</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_1</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_2</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_3</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_4</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_5</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_7</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_8</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_9</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_10</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_11</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_12</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_13</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_14</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_15</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_16</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_17</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_18</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_19</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_20</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_21</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_22</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_23</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_24</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_25</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_26</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_27</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_28</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_29</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6I_30</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_1</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_2</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_3</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_4</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_5</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_6</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_7</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_8</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_9</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_10</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_11</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_12</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_13</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_14</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_15</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_16</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_17</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_18</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_19</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_20</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_21</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_22</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_23</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_24</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_25</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_26</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_27</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_28</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_29</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6II_30</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_1</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_2</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_3</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_4</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_5</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_6</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_7</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_8</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_9</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_10</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_11</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_12</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_13</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_14</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_15</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_16</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_17</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_18</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_19</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_20</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_21</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_22</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_23</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_24</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_25</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_26</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_27</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_28</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_29</t>
+  </si>
+  <si>
+    <t>benchmarks_triboringC6III_30</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_1</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_2</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_3</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_4</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_5</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_6</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_7</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_8</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_9</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_10</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_11</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_12</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_13</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_14</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_15</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_16</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_17</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_18</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_19</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_20</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_21</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_22</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_23</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_24</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_25</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_26</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_27</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_28</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_29</t>
+  </si>
+  <si>
+    <t>benchmarks_perlitev2_30</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_1</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_2</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_3</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_4</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_5</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_6</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_7</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_8</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_9</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_10</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_11</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_12</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_13</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_14</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_15</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_16</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_17</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_18</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_19</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_20</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_21</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_22</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_23</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_24</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_25</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_26</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_27</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_28</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_29</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv2_30</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_1</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_2</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_3</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_4</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_5</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_6</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_7</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_8</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_9</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_10</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_11</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_12</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_13</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_14</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_15</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_16</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_17</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_18</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_19</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_20</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_21</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_22</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_23</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_24</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_25</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_26</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_27</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_28</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_29</t>
+  </si>
+  <si>
+    <t>benchmarks_otherWEL_30</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_1</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_2</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_3</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_4</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_5</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_6</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_7</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_8</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_9</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_10</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_11</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_12</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_13</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_14</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_15</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_16</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_17</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_18</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_19</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_20</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_21</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_22</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_23</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_24</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_25</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_26</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_27</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_28</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_29</t>
+  </si>
+  <si>
+    <t>benchmarks_WELv3_30</t>
   </si>
 </sst>
 </file>
@@ -1467,10 +2676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N55"/>
+  <dimension ref="B1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="O49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R71" sqref="R71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1483,11 +2692,18 @@
     <col min="7" max="7" width="29.1796875" customWidth="1"/>
     <col min="8" max="8" width="26.7265625" customWidth="1"/>
     <col min="9" max="9" width="21.54296875" customWidth="1"/>
-    <col min="10" max="10" width="21.26953125" customWidth="1"/>
-    <col min="11" max="11" width="20.7265625" customWidth="1"/>
-    <col min="12" max="12" width="17.453125" customWidth="1"/>
-    <col min="13" max="13" width="18.54296875" customWidth="1"/>
-    <col min="14" max="14" width="12.54296875" customWidth="1"/>
+    <col min="10" max="10" width="28.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.1796875" customWidth="1"/>
+    <col min="12" max="12" width="34.81640625" customWidth="1"/>
+    <col min="13" max="13" width="39.453125" customWidth="1"/>
+    <col min="14" max="14" width="34.26953125" customWidth="1"/>
+    <col min="15" max="15" width="29.90625" customWidth="1"/>
+    <col min="16" max="16" width="26.26953125" customWidth="1"/>
+    <col min="17" max="17" width="29" customWidth="1"/>
+    <col min="18" max="18" width="33.81640625" customWidth="1"/>
+    <col min="19" max="19" width="24.81640625" customWidth="1"/>
+    <col min="20" max="20" width="23.90625" customWidth="1"/>
+    <col min="21" max="21" width="30.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.35">
@@ -2319,6 +3535,9 @@
       <c r="G28" t="s">
         <v>345</v>
       </c>
+      <c r="H28" t="s">
+        <v>373</v>
+      </c>
       <c r="K28" t="s">
         <v>135</v>
       </c>
@@ -2342,6 +3561,9 @@
       <c r="G29" t="s">
         <v>346</v>
       </c>
+      <c r="H29" t="s">
+        <v>374</v>
+      </c>
       <c r="K29" t="s">
         <v>136</v>
       </c>
@@ -2362,6 +3584,9 @@
       <c r="G30" t="s">
         <v>347</v>
       </c>
+      <c r="H30" t="s">
+        <v>375</v>
+      </c>
       <c r="K30" t="s">
         <v>137</v>
       </c>
@@ -2382,6 +3607,9 @@
       <c r="G31" t="s">
         <v>348</v>
       </c>
+      <c r="H31" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
@@ -2396,8 +3624,11 @@
       <c r="G32" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>260</v>
       </c>
@@ -2410,8 +3641,11 @@
       <c r="G33" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>261</v>
       </c>
@@ -2424,8 +3658,11 @@
       <c r="G34" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>271</v>
       </c>
@@ -2438,8 +3675,11 @@
       <c r="G35" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>273</v>
       </c>
@@ -2452,8 +3692,11 @@
       <c r="G36" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H36" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>274</v>
       </c>
@@ -2466,8 +3709,11 @@
       <c r="G37" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H37" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>275</v>
       </c>
@@ -2480,8 +3726,11 @@
       <c r="G38" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H38" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>276</v>
       </c>
@@ -2494,8 +3743,11 @@
       <c r="G39" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H39" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>277</v>
       </c>
@@ -2508,8 +3760,11 @@
       <c r="G40" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H40" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>278</v>
       </c>
@@ -2522,8 +3777,11 @@
       <c r="G41" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H41" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>279</v>
       </c>
@@ -2536,8 +3794,11 @@
       <c r="G42" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H42" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>280</v>
       </c>
@@ -2550,8 +3811,11 @@
       <c r="G43" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H43" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>281</v>
       </c>
@@ -2564,8 +3828,11 @@
       <c r="G44" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H44" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>282</v>
       </c>
@@ -2578,8 +3845,11 @@
       <c r="G45" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H45" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>283</v>
       </c>
@@ -2592,8 +3862,11 @@
       <c r="G46" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H46" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>284</v>
       </c>
@@ -2606,8 +3879,11 @@
       <c r="G47" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H47" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>285</v>
       </c>
@@ -2620,8 +3896,11 @@
       <c r="G48" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H48" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="49" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>286</v>
       </c>
@@ -2634,8 +3913,11 @@
       <c r="G49" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H49" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="50" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>287</v>
       </c>
@@ -2648,8 +3930,11 @@
       <c r="G50" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H50" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="51" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>288</v>
       </c>
@@ -2662,8 +3947,47 @@
       <c r="G51" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H51" t="s">
+        <v>396</v>
+      </c>
+      <c r="J51" t="s">
+        <v>416</v>
+      </c>
+      <c r="K51" t="s">
+        <v>446</v>
+      </c>
+      <c r="L51" t="s">
+        <v>477</v>
+      </c>
+      <c r="M51" t="s">
+        <v>507</v>
+      </c>
+      <c r="N51" t="s">
+        <v>537</v>
+      </c>
+      <c r="O51" t="s">
+        <v>567</v>
+      </c>
+      <c r="P51" t="s">
+        <v>596</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>626</v>
+      </c>
+      <c r="R51" t="s">
+        <v>656</v>
+      </c>
+      <c r="S51" t="s">
+        <v>686</v>
+      </c>
+      <c r="T51" t="s">
+        <v>716</v>
+      </c>
+      <c r="U51" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="52" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>289</v>
       </c>
@@ -2676,8 +4000,47 @@
       <c r="G52" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H52" t="s">
+        <v>397</v>
+      </c>
+      <c r="J52" t="s">
+        <v>417</v>
+      </c>
+      <c r="K52" t="s">
+        <v>448</v>
+      </c>
+      <c r="L52" t="s">
+        <v>478</v>
+      </c>
+      <c r="M52" t="s">
+        <v>508</v>
+      </c>
+      <c r="N52" t="s">
+        <v>538</v>
+      </c>
+      <c r="O52" t="s">
+        <v>568</v>
+      </c>
+      <c r="P52" t="s">
+        <v>597</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>627</v>
+      </c>
+      <c r="R52" t="s">
+        <v>657</v>
+      </c>
+      <c r="S52" t="s">
+        <v>687</v>
+      </c>
+      <c r="T52" t="s">
+        <v>717</v>
+      </c>
+      <c r="U52" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="53" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>290</v>
       </c>
@@ -2690,8 +4053,47 @@
       <c r="G53" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H53" t="s">
+        <v>398</v>
+      </c>
+      <c r="J53" t="s">
+        <v>418</v>
+      </c>
+      <c r="K53" t="s">
+        <v>449</v>
+      </c>
+      <c r="L53" t="s">
+        <v>479</v>
+      </c>
+      <c r="M53" t="s">
+        <v>509</v>
+      </c>
+      <c r="N53" t="s">
+        <v>539</v>
+      </c>
+      <c r="O53" t="s">
+        <v>569</v>
+      </c>
+      <c r="P53" t="s">
+        <v>598</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>628</v>
+      </c>
+      <c r="R53" t="s">
+        <v>658</v>
+      </c>
+      <c r="S53" t="s">
+        <v>688</v>
+      </c>
+      <c r="T53" t="s">
+        <v>718</v>
+      </c>
+      <c r="U53" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="54" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>291</v>
       </c>
@@ -2704,8 +4106,47 @@
       <c r="G54" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="H54" t="s">
+        <v>399</v>
+      </c>
+      <c r="J54" t="s">
+        <v>419</v>
+      </c>
+      <c r="K54" t="s">
+        <v>450</v>
+      </c>
+      <c r="L54" t="s">
+        <v>480</v>
+      </c>
+      <c r="M54" t="s">
+        <v>510</v>
+      </c>
+      <c r="N54" t="s">
+        <v>540</v>
+      </c>
+      <c r="O54" t="s">
+        <v>570</v>
+      </c>
+      <c r="P54" t="s">
+        <v>599</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>629</v>
+      </c>
+      <c r="R54" t="s">
+        <v>659</v>
+      </c>
+      <c r="S54" t="s">
+        <v>689</v>
+      </c>
+      <c r="T54" t="s">
+        <v>719</v>
+      </c>
+      <c r="U54" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>292</v>
       </c>
@@ -2717,11 +4158,1045 @@
       </c>
       <c r="G55" t="s">
         <v>372</v>
+      </c>
+      <c r="H55" t="s">
+        <v>400</v>
+      </c>
+      <c r="J55" t="s">
+        <v>420</v>
+      </c>
+      <c r="K55" t="s">
+        <v>451</v>
+      </c>
+      <c r="L55" t="s">
+        <v>481</v>
+      </c>
+      <c r="M55" t="s">
+        <v>511</v>
+      </c>
+      <c r="N55" t="s">
+        <v>541</v>
+      </c>
+      <c r="O55" t="s">
+        <v>571</v>
+      </c>
+      <c r="P55" t="s">
+        <v>600</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>630</v>
+      </c>
+      <c r="R55" t="s">
+        <v>660</v>
+      </c>
+      <c r="S55" t="s">
+        <v>690</v>
+      </c>
+      <c r="T55" t="s">
+        <v>720</v>
+      </c>
+      <c r="U55" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="H56" t="s">
+        <v>401</v>
+      </c>
+      <c r="J56" t="s">
+        <v>421</v>
+      </c>
+      <c r="K56" t="s">
+        <v>452</v>
+      </c>
+      <c r="L56" t="s">
+        <v>482</v>
+      </c>
+      <c r="M56" t="s">
+        <v>512</v>
+      </c>
+      <c r="N56" t="s">
+        <v>542</v>
+      </c>
+      <c r="O56" t="s">
+        <v>447</v>
+      </c>
+      <c r="P56" t="s">
+        <v>601</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>631</v>
+      </c>
+      <c r="R56" t="s">
+        <v>661</v>
+      </c>
+      <c r="S56" t="s">
+        <v>691</v>
+      </c>
+      <c r="T56" t="s">
+        <v>721</v>
+      </c>
+      <c r="U56" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="57" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="H57" t="s">
+        <v>402</v>
+      </c>
+      <c r="J57" t="s">
+        <v>422</v>
+      </c>
+      <c r="K57" t="s">
+        <v>453</v>
+      </c>
+      <c r="L57" t="s">
+        <v>483</v>
+      </c>
+      <c r="M57" t="s">
+        <v>513</v>
+      </c>
+      <c r="N57" t="s">
+        <v>543</v>
+      </c>
+      <c r="O57" t="s">
+        <v>572</v>
+      </c>
+      <c r="P57" t="s">
+        <v>602</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>632</v>
+      </c>
+      <c r="R57" t="s">
+        <v>662</v>
+      </c>
+      <c r="S57" t="s">
+        <v>692</v>
+      </c>
+      <c r="T57" t="s">
+        <v>722</v>
+      </c>
+      <c r="U57" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="58" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="H58" t="s">
+        <v>403</v>
+      </c>
+      <c r="J58" t="s">
+        <v>423</v>
+      </c>
+      <c r="K58" t="s">
+        <v>454</v>
+      </c>
+      <c r="L58" t="s">
+        <v>484</v>
+      </c>
+      <c r="M58" t="s">
+        <v>514</v>
+      </c>
+      <c r="N58" t="s">
+        <v>544</v>
+      </c>
+      <c r="O58" t="s">
+        <v>573</v>
+      </c>
+      <c r="P58" t="s">
+        <v>603</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>633</v>
+      </c>
+      <c r="R58" t="s">
+        <v>663</v>
+      </c>
+      <c r="S58" t="s">
+        <v>693</v>
+      </c>
+      <c r="T58" t="s">
+        <v>723</v>
+      </c>
+      <c r="U58" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="59" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="H59" t="s">
+        <v>404</v>
+      </c>
+      <c r="J59" t="s">
+        <v>424</v>
+      </c>
+      <c r="K59" t="s">
+        <v>455</v>
+      </c>
+      <c r="L59" t="s">
+        <v>485</v>
+      </c>
+      <c r="M59" t="s">
+        <v>515</v>
+      </c>
+      <c r="N59" t="s">
+        <v>545</v>
+      </c>
+      <c r="O59" t="s">
+        <v>574</v>
+      </c>
+      <c r="P59" t="s">
+        <v>604</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>634</v>
+      </c>
+      <c r="R59" t="s">
+        <v>664</v>
+      </c>
+      <c r="S59" t="s">
+        <v>694</v>
+      </c>
+      <c r="T59" t="s">
+        <v>724</v>
+      </c>
+      <c r="U59" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="60" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="H60" t="s">
+        <v>405</v>
+      </c>
+      <c r="J60" t="s">
+        <v>425</v>
+      </c>
+      <c r="K60" t="s">
+        <v>456</v>
+      </c>
+      <c r="L60" t="s">
+        <v>486</v>
+      </c>
+      <c r="M60" t="s">
+        <v>516</v>
+      </c>
+      <c r="N60" t="s">
+        <v>546</v>
+      </c>
+      <c r="O60" t="s">
+        <v>575</v>
+      </c>
+      <c r="P60" t="s">
+        <v>605</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>635</v>
+      </c>
+      <c r="R60" t="s">
+        <v>665</v>
+      </c>
+      <c r="S60" t="s">
+        <v>695</v>
+      </c>
+      <c r="T60" t="s">
+        <v>725</v>
+      </c>
+      <c r="U60" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="61" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="H61" t="s">
+        <v>406</v>
+      </c>
+      <c r="J61" t="s">
+        <v>426</v>
+      </c>
+      <c r="K61" t="s">
+        <v>457</v>
+      </c>
+      <c r="L61" t="s">
+        <v>487</v>
+      </c>
+      <c r="M61" t="s">
+        <v>517</v>
+      </c>
+      <c r="N61" t="s">
+        <v>547</v>
+      </c>
+      <c r="O61" t="s">
+        <v>576</v>
+      </c>
+      <c r="P61" t="s">
+        <v>606</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>636</v>
+      </c>
+      <c r="R61" t="s">
+        <v>666</v>
+      </c>
+      <c r="S61" t="s">
+        <v>696</v>
+      </c>
+      <c r="T61" t="s">
+        <v>726</v>
+      </c>
+      <c r="U61" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="H62" t="s">
+        <v>407</v>
+      </c>
+      <c r="J62" t="s">
+        <v>427</v>
+      </c>
+      <c r="K62" t="s">
+        <v>458</v>
+      </c>
+      <c r="L62" t="s">
+        <v>488</v>
+      </c>
+      <c r="M62" t="s">
+        <v>518</v>
+      </c>
+      <c r="N62" t="s">
+        <v>548</v>
+      </c>
+      <c r="O62" t="s">
+        <v>577</v>
+      </c>
+      <c r="P62" t="s">
+        <v>607</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>637</v>
+      </c>
+      <c r="R62" t="s">
+        <v>667</v>
+      </c>
+      <c r="S62" t="s">
+        <v>697</v>
+      </c>
+      <c r="T62" t="s">
+        <v>727</v>
+      </c>
+      <c r="U62" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="63" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="H63" t="s">
+        <v>408</v>
+      </c>
+      <c r="J63" t="s">
+        <v>428</v>
+      </c>
+      <c r="K63" t="s">
+        <v>459</v>
+      </c>
+      <c r="L63" t="s">
+        <v>489</v>
+      </c>
+      <c r="M63" t="s">
+        <v>519</v>
+      </c>
+      <c r="N63" t="s">
+        <v>549</v>
+      </c>
+      <c r="O63" t="s">
+        <v>578</v>
+      </c>
+      <c r="P63" t="s">
+        <v>608</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>638</v>
+      </c>
+      <c r="R63" t="s">
+        <v>668</v>
+      </c>
+      <c r="S63" t="s">
+        <v>698</v>
+      </c>
+      <c r="T63" t="s">
+        <v>728</v>
+      </c>
+      <c r="U63" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="64" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="H64" t="s">
+        <v>409</v>
+      </c>
+      <c r="J64" t="s">
+        <v>429</v>
+      </c>
+      <c r="K64" t="s">
+        <v>460</v>
+      </c>
+      <c r="L64" t="s">
+        <v>490</v>
+      </c>
+      <c r="M64" t="s">
+        <v>520</v>
+      </c>
+      <c r="N64" t="s">
+        <v>550</v>
+      </c>
+      <c r="O64" t="s">
+        <v>579</v>
+      </c>
+      <c r="P64" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>639</v>
+      </c>
+      <c r="R64" t="s">
+        <v>669</v>
+      </c>
+      <c r="S64" t="s">
+        <v>699</v>
+      </c>
+      <c r="T64" t="s">
+        <v>729</v>
+      </c>
+      <c r="U64" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="65" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="H65" t="s">
+        <v>410</v>
+      </c>
+      <c r="J65" t="s">
+        <v>430</v>
+      </c>
+      <c r="K65" t="s">
+        <v>461</v>
+      </c>
+      <c r="L65" t="s">
+        <v>491</v>
+      </c>
+      <c r="M65" t="s">
+        <v>521</v>
+      </c>
+      <c r="N65" t="s">
+        <v>551</v>
+      </c>
+      <c r="O65" t="s">
+        <v>580</v>
+      </c>
+      <c r="P65" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>640</v>
+      </c>
+      <c r="R65" t="s">
+        <v>670</v>
+      </c>
+      <c r="S65" t="s">
+        <v>700</v>
+      </c>
+      <c r="T65" t="s">
+        <v>730</v>
+      </c>
+      <c r="U65" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="66" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="H66" t="s">
+        <v>411</v>
+      </c>
+      <c r="J66" t="s">
+        <v>431</v>
+      </c>
+      <c r="K66" t="s">
+        <v>462</v>
+      </c>
+      <c r="L66" t="s">
+        <v>492</v>
+      </c>
+      <c r="M66" t="s">
+        <v>522</v>
+      </c>
+      <c r="N66" t="s">
+        <v>552</v>
+      </c>
+      <c r="O66" t="s">
+        <v>581</v>
+      </c>
+      <c r="P66" t="s">
+        <v>611</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>641</v>
+      </c>
+      <c r="R66" t="s">
+        <v>671</v>
+      </c>
+      <c r="S66" t="s">
+        <v>701</v>
+      </c>
+      <c r="T66" t="s">
+        <v>731</v>
+      </c>
+      <c r="U66" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="67" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="H67" t="s">
+        <v>412</v>
+      </c>
+      <c r="J67" t="s">
+        <v>432</v>
+      </c>
+      <c r="K67" t="s">
+        <v>463</v>
+      </c>
+      <c r="L67" t="s">
+        <v>493</v>
+      </c>
+      <c r="M67" t="s">
+        <v>523</v>
+      </c>
+      <c r="N67" t="s">
+        <v>553</v>
+      </c>
+      <c r="O67" t="s">
+        <v>582</v>
+      </c>
+      <c r="P67" t="s">
+        <v>612</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>642</v>
+      </c>
+      <c r="R67" t="s">
+        <v>672</v>
+      </c>
+      <c r="S67" t="s">
+        <v>702</v>
+      </c>
+      <c r="T67" t="s">
+        <v>732</v>
+      </c>
+      <c r="U67" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="68" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="H68" t="s">
+        <v>413</v>
+      </c>
+      <c r="J68" t="s">
+        <v>433</v>
+      </c>
+      <c r="K68" t="s">
+        <v>464</v>
+      </c>
+      <c r="L68" t="s">
+        <v>494</v>
+      </c>
+      <c r="M68" t="s">
+        <v>524</v>
+      </c>
+      <c r="N68" t="s">
+        <v>554</v>
+      </c>
+      <c r="O68" t="s">
+        <v>583</v>
+      </c>
+      <c r="P68" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>643</v>
+      </c>
+      <c r="R68" t="s">
+        <v>673</v>
+      </c>
+      <c r="S68" t="s">
+        <v>703</v>
+      </c>
+      <c r="T68" t="s">
+        <v>733</v>
+      </c>
+      <c r="U68" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="69" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="H69" t="s">
+        <v>414</v>
+      </c>
+      <c r="J69" t="s">
+        <v>434</v>
+      </c>
+      <c r="K69" t="s">
+        <v>465</v>
+      </c>
+      <c r="L69" t="s">
+        <v>495</v>
+      </c>
+      <c r="M69" t="s">
+        <v>525</v>
+      </c>
+      <c r="N69" t="s">
+        <v>555</v>
+      </c>
+      <c r="O69" t="s">
+        <v>584</v>
+      </c>
+      <c r="P69" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>644</v>
+      </c>
+      <c r="R69" t="s">
+        <v>674</v>
+      </c>
+      <c r="S69" t="s">
+        <v>704</v>
+      </c>
+      <c r="T69" t="s">
+        <v>734</v>
+      </c>
+      <c r="U69" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="70" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="H70" t="s">
+        <v>415</v>
+      </c>
+      <c r="J70" t="s">
+        <v>435</v>
+      </c>
+      <c r="K70" t="s">
+        <v>466</v>
+      </c>
+      <c r="L70" t="s">
+        <v>496</v>
+      </c>
+      <c r="M70" t="s">
+        <v>526</v>
+      </c>
+      <c r="N70" t="s">
+        <v>556</v>
+      </c>
+      <c r="O70" t="s">
+        <v>585</v>
+      </c>
+      <c r="P70" t="s">
+        <v>615</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>645</v>
+      </c>
+      <c r="R70" t="s">
+        <v>675</v>
+      </c>
+      <c r="S70" t="s">
+        <v>705</v>
+      </c>
+      <c r="T70" t="s">
+        <v>735</v>
+      </c>
+      <c r="U70" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="71" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="J71" t="s">
+        <v>436</v>
+      </c>
+      <c r="K71" t="s">
+        <v>467</v>
+      </c>
+      <c r="L71" t="s">
+        <v>497</v>
+      </c>
+      <c r="M71" t="s">
+        <v>527</v>
+      </c>
+      <c r="N71" t="s">
+        <v>557</v>
+      </c>
+      <c r="O71" t="s">
+        <v>586</v>
+      </c>
+      <c r="P71" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>646</v>
+      </c>
+      <c r="R71" t="s">
+        <v>676</v>
+      </c>
+      <c r="S71" t="s">
+        <v>706</v>
+      </c>
+      <c r="T71" t="s">
+        <v>736</v>
+      </c>
+      <c r="U71" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="72" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="J72" t="s">
+        <v>437</v>
+      </c>
+      <c r="K72" t="s">
+        <v>468</v>
+      </c>
+      <c r="L72" t="s">
+        <v>498</v>
+      </c>
+      <c r="M72" t="s">
+        <v>528</v>
+      </c>
+      <c r="N72" t="s">
+        <v>558</v>
+      </c>
+      <c r="O72" t="s">
+        <v>587</v>
+      </c>
+      <c r="P72" t="s">
+        <v>617</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>647</v>
+      </c>
+      <c r="R72" t="s">
+        <v>677</v>
+      </c>
+      <c r="S72" t="s">
+        <v>707</v>
+      </c>
+      <c r="T72" t="s">
+        <v>737</v>
+      </c>
+      <c r="U72" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="73" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="J73" t="s">
+        <v>438</v>
+      </c>
+      <c r="K73" t="s">
+        <v>469</v>
+      </c>
+      <c r="L73" t="s">
+        <v>499</v>
+      </c>
+      <c r="M73" t="s">
+        <v>529</v>
+      </c>
+      <c r="N73" t="s">
+        <v>559</v>
+      </c>
+      <c r="O73" t="s">
+        <v>588</v>
+      </c>
+      <c r="P73" t="s">
+        <v>618</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>648</v>
+      </c>
+      <c r="R73" t="s">
+        <v>678</v>
+      </c>
+      <c r="S73" t="s">
+        <v>708</v>
+      </c>
+      <c r="T73" t="s">
+        <v>738</v>
+      </c>
+      <c r="U73" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="74" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="J74" t="s">
+        <v>439</v>
+      </c>
+      <c r="K74" t="s">
+        <v>470</v>
+      </c>
+      <c r="L74" t="s">
+        <v>500</v>
+      </c>
+      <c r="M74" t="s">
+        <v>530</v>
+      </c>
+      <c r="N74" t="s">
+        <v>560</v>
+      </c>
+      <c r="O74" t="s">
+        <v>589</v>
+      </c>
+      <c r="P74" t="s">
+        <v>619</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>649</v>
+      </c>
+      <c r="R74" t="s">
+        <v>679</v>
+      </c>
+      <c r="S74" t="s">
+        <v>709</v>
+      </c>
+      <c r="T74" t="s">
+        <v>739</v>
+      </c>
+      <c r="U74" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="75" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="J75" t="s">
+        <v>440</v>
+      </c>
+      <c r="K75" t="s">
+        <v>471</v>
+      </c>
+      <c r="L75" t="s">
+        <v>501</v>
+      </c>
+      <c r="M75" t="s">
+        <v>531</v>
+      </c>
+      <c r="N75" t="s">
+        <v>561</v>
+      </c>
+      <c r="O75" t="s">
+        <v>590</v>
+      </c>
+      <c r="P75" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>650</v>
+      </c>
+      <c r="R75" t="s">
+        <v>680</v>
+      </c>
+      <c r="S75" t="s">
+        <v>710</v>
+      </c>
+      <c r="T75" t="s">
+        <v>740</v>
+      </c>
+      <c r="U75" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="76" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="J76" t="s">
+        <v>441</v>
+      </c>
+      <c r="K76" t="s">
+        <v>472</v>
+      </c>
+      <c r="L76" t="s">
+        <v>502</v>
+      </c>
+      <c r="M76" t="s">
+        <v>532</v>
+      </c>
+      <c r="N76" t="s">
+        <v>562</v>
+      </c>
+      <c r="O76" t="s">
+        <v>591</v>
+      </c>
+      <c r="P76" t="s">
+        <v>621</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>651</v>
+      </c>
+      <c r="R76" t="s">
+        <v>681</v>
+      </c>
+      <c r="S76" t="s">
+        <v>711</v>
+      </c>
+      <c r="T76" t="s">
+        <v>741</v>
+      </c>
+      <c r="U76" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="77" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="J77" t="s">
+        <v>442</v>
+      </c>
+      <c r="K77" t="s">
+        <v>473</v>
+      </c>
+      <c r="L77" t="s">
+        <v>503</v>
+      </c>
+      <c r="M77" t="s">
+        <v>533</v>
+      </c>
+      <c r="N77" t="s">
+        <v>563</v>
+      </c>
+      <c r="O77" t="s">
+        <v>592</v>
+      </c>
+      <c r="P77" t="s">
+        <v>622</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>652</v>
+      </c>
+      <c r="R77" t="s">
+        <v>682</v>
+      </c>
+      <c r="S77" t="s">
+        <v>712</v>
+      </c>
+      <c r="T77" t="s">
+        <v>742</v>
+      </c>
+      <c r="U77" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="78" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="J78" t="s">
+        <v>443</v>
+      </c>
+      <c r="K78" t="s">
+        <v>474</v>
+      </c>
+      <c r="L78" t="s">
+        <v>504</v>
+      </c>
+      <c r="M78" t="s">
+        <v>534</v>
+      </c>
+      <c r="N78" t="s">
+        <v>564</v>
+      </c>
+      <c r="O78" t="s">
+        <v>593</v>
+      </c>
+      <c r="P78" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>653</v>
+      </c>
+      <c r="R78" t="s">
+        <v>683</v>
+      </c>
+      <c r="S78" t="s">
+        <v>713</v>
+      </c>
+      <c r="T78" t="s">
+        <v>743</v>
+      </c>
+      <c r="U78" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="79" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="J79" t="s">
+        <v>444</v>
+      </c>
+      <c r="K79" t="s">
+        <v>475</v>
+      </c>
+      <c r="L79" t="s">
+        <v>505</v>
+      </c>
+      <c r="M79" t="s">
+        <v>535</v>
+      </c>
+      <c r="N79" t="s">
+        <v>565</v>
+      </c>
+      <c r="O79" t="s">
+        <v>594</v>
+      </c>
+      <c r="P79" t="s">
+        <v>624</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>654</v>
+      </c>
+      <c r="R79" t="s">
+        <v>684</v>
+      </c>
+      <c r="S79" t="s">
+        <v>714</v>
+      </c>
+      <c r="T79" t="s">
+        <v>744</v>
+      </c>
+      <c r="U79" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="80" spans="8:21" x14ac:dyDescent="0.35">
+      <c r="J80" t="s">
+        <v>445</v>
+      </c>
+      <c r="K80" t="s">
+        <v>476</v>
+      </c>
+      <c r="L80" t="s">
+        <v>506</v>
+      </c>
+      <c r="M80" t="s">
+        <v>536</v>
+      </c>
+      <c r="N80" t="s">
+        <v>566</v>
+      </c>
+      <c r="O80" t="s">
+        <v>595</v>
+      </c>
+      <c r="P80" t="s">
+        <v>625</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>655</v>
+      </c>
+      <c r="R80" t="s">
+        <v>685</v>
+      </c>
+      <c r="S80" t="s">
+        <v>715</v>
+      </c>
+      <c r="T80" t="s">
+        <v>745</v>
+      </c>
+      <c r="U80" t="s">
+        <v>775</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>